<commit_message>
Adding first parameter and dataset for analysis
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salazad4\Code\ArrayoConsulting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salazad4\Code\Arrayo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A65F1EED-029A-4AE4-8D43-CF649B440210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B016E5-F0A9-450F-BBE8-EBF2EEE0A655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C251713C-BB1E-455F-8E5E-77CA242A37D5}"/>
   </bookViews>
@@ -17,21 +17,9 @@
     <sheet name="Param2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -41,9 +29,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="10">
   <si>
     <t>Group</t>
-  </si>
-  <si>
-    <t>Animal  ID</t>
   </si>
   <si>
     <t>Placebo</t>
@@ -64,10 +49,13 @@
     <t>Animal _ID</t>
   </si>
   <si>
-    <t>Parameter1-0h</t>
+    <t>Animal_ID</t>
   </si>
   <si>
-    <t>Parameter1-12h</t>
+    <t>Parameter1_0h</t>
+  </si>
+  <si>
+    <t>Parameter1_12h</t>
   </si>
 </sst>
 </file>
@@ -496,7 +484,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +494,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
@@ -517,7 +505,7 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -531,7 +519,7 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -545,7 +533,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -559,7 +547,7 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -573,7 +561,7 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -587,7 +575,7 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -601,7 +589,7 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -615,7 +603,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -629,7 +617,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -643,7 +631,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" s="3">
         <v>10</v>
@@ -657,7 +645,7 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" s="3">
         <v>11</v>
@@ -671,7 +659,7 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="3">
         <v>12</v>
@@ -685,7 +673,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="3">
         <v>13</v>
@@ -699,7 +687,7 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="3">
         <v>14</v>
@@ -713,7 +701,7 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" s="3">
         <v>15</v>
@@ -727,7 +715,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="3">
         <v>16</v>
@@ -741,7 +729,7 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="3">
         <v>17</v>
@@ -755,7 +743,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="3">
         <v>18</v>
@@ -769,7 +757,7 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="3">
         <v>19</v>
@@ -783,7 +771,7 @@
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="3">
         <v>20</v>
@@ -797,7 +785,7 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="3">
         <v>21</v>
@@ -811,7 +799,7 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="3">
         <v>22</v>
@@ -825,7 +813,7 @@
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" s="3">
         <v>23</v>
@@ -839,7 +827,7 @@
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="3">
         <v>24</v>
@@ -872,15 +860,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -891,7 +879,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -902,7 +890,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -913,7 +901,7 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -924,7 +912,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
@@ -935,7 +923,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
@@ -946,7 +934,7 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
@@ -957,7 +945,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
@@ -968,7 +956,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
@@ -979,7 +967,7 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" s="3">
         <v>10</v>
@@ -990,7 +978,7 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" s="3">
         <v>11</v>
@@ -1001,7 +989,7 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="3">
         <v>12</v>
@@ -1012,7 +1000,7 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="3">
         <v>13</v>
@@ -1023,7 +1011,7 @@
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="3">
         <v>14</v>
@@ -1034,7 +1022,7 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" s="3">
         <v>15</v>
@@ -1045,7 +1033,7 @@
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="3">
         <v>16</v>
@@ -1056,7 +1044,7 @@
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="3">
         <v>17</v>
@@ -1067,7 +1055,7 @@
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="3">
         <v>18</v>
@@ -1078,7 +1066,7 @@
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="3">
         <v>19</v>
@@ -1089,7 +1077,7 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="3">
         <v>20</v>
@@ -1100,7 +1088,7 @@
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="3">
         <v>21</v>
@@ -1111,7 +1099,7 @@
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="3">
         <v>22</v>
@@ -1122,7 +1110,7 @@
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" s="3">
         <v>23</v>
@@ -1133,7 +1121,7 @@
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="3">
         <v>24</v>

</xml_diff>